<commit_message>
add reward and agent final adjustments
</commit_message>
<xml_diff>
--- a/config_file.xlsx
+++ b/config_file.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erez/Documents/Project_B/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erez/PycharmProjects/Project_B/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86B508D-1B81-3B4E-AAE5-891A8960825B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6FC750D-A50E-1141-9C2A-6E9C6D77D757}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14000" yWindow="9560" windowWidth="21680" windowHeight="10960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16720" yWindow="3220" windowWidth="21680" windowHeight="10960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hyperparameters" sheetId="1" r:id="rId1"/>
@@ -544,7 +544,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="167" zoomScaleNormal="167" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -600,7 +600,7 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -648,7 +648,7 @@
         <v>32</v>
       </c>
       <c r="B11">
-        <v>100</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -687,7 +687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView zoomScale="198" zoomScaleNormal="198" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="198" zoomScaleNormal="198" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>

</xml_diff>